<commit_message>
FINAL FIX: Resolved subprocess path duplication error (Error 2) and confirmed permissions (Error 1).
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\Sunday Football\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\To upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653A20C6-0B4E-41F9-A2EC-7B03638264F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3C6996-E5E7-46FF-877B-3473598BE43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division 1" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -222,7 +222,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -624,7 +623,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,8 +657,12 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2" t="s">
         <v>37</v>
       </c>
@@ -690,7 +693,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -724,6 +727,12 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
@@ -731,6 +740,12 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -753,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,6 +807,12 @@
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
@@ -803,8 +824,12 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
@@ -816,6 +841,12 @@
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
@@ -827,6 +858,12 @@
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
@@ -838,7 +875,12 @@
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
@@ -850,6 +892,12 @@
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
@@ -862,7 +910,12 @@
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
@@ -874,6 +927,12 @@
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
@@ -885,7 +944,12 @@
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
@@ -897,6 +961,12 @@
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
@@ -908,6 +978,12 @@
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
@@ -919,7 +995,12 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
@@ -930,6 +1011,12 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>36</v>

</xml_diff>